<commit_message>
handle personid missing issue
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X36"/>
+  <dimension ref="A1:X65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,16 +557,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>67522</v>
+        <v>67558</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>定舫詩紀</t>
+          <t>水香園詩稿</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ding fang shi ji</t>
+          <t>shui xiang yuan shi gao</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
@@ -581,7 +581,7 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K2" t="inlineStr"/>
@@ -608,7 +608,7 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V2" t="inlineStr"/>
@@ -617,16 +617,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>67523</v>
+        <v>67559</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>韻閣詩: 十卷</t>
+          <t>冶城游草</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>yun ge shi</t>
+          <t>ye cheng you cao</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -641,7 +641,7 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K3" t="inlineStr"/>
@@ -668,7 +668,7 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V3" t="inlineStr"/>
@@ -677,16 +677,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>67524</v>
+        <v>67560</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>茶園詩: 十卷</t>
+          <t>滋蘭堂集</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>cha yuan shi</t>
+          <t>zi lan tang ji</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -701,7 +701,7 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K4" t="inlineStr"/>
@@ -728,7 +728,7 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V4" t="inlineStr"/>
@@ -737,16 +737,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>67525</v>
+        <v>67561</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>練江詩鈔</t>
+          <t>續黃山志</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>lian jiang shi chao</t>
+          <t>xu huang shan zhi</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
@@ -788,7 +788,7 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V5" t="inlineStr"/>
@@ -797,16 +797,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>67526</v>
+        <v>67562</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>含翠樓詩文集</t>
+          <t>七峯草堂詩稿: 十卷</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>han cui lou shi wen ji</t>
+          <t>qi feng cao tang shi gao</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
@@ -848,7 +848,7 @@
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V6" t="inlineStr"/>
@@ -857,16 +857,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>67527</v>
+        <v>67563</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>稽古堂詩: 六卷</t>
+          <t>紅藥書莊詩</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ji gu tang shi</t>
+          <t>hong yao shu zhuang shi</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -908,7 +908,7 @@
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V7" t="inlineStr"/>
@@ -917,16 +917,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>67528</v>
+        <v>67564</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>自怡草</t>
+          <t>半舫齋稾</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>zi yi cao</t>
+          <t>ban fang zhai gao</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
@@ -941,7 +941,7 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K8" t="inlineStr"/>
@@ -968,7 +968,7 @@
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V8" t="inlineStr"/>
@@ -977,16 +977,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>67529</v>
+        <v>67565</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>歷畊草</t>
+          <t>用餘堂集</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>li geng cao</t>
+          <t>yong yu tang ji</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V9" t="inlineStr"/>
@@ -1037,16 +1037,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>67530</v>
+        <v>67566</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>小巢湖詩</t>
+          <t>若菴集</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>xiao chao hu shi</t>
+          <t>ruo an ji</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
@@ -1061,7 +1061,7 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K10" t="inlineStr"/>
@@ -1088,7 +1088,7 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V10" t="inlineStr"/>
@@ -1097,16 +1097,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>67531</v>
+        <v>67567</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>秋水晚山樓詩集</t>
+          <t>儷體文鈔</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>qiu shui wan shan lou shi ji</t>
+          <t>li ti wen chao</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
@@ -1121,7 +1121,7 @@
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K11" t="inlineStr"/>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V11" t="inlineStr"/>
@@ -1157,16 +1157,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>67532</v>
+        <v>67568</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>廣陵擪笛詞: 一卷</t>
+          <t>昭明詩選輯注</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>guang ling ye di ci</t>
+          <t>zhao ming shi xuan ji zhu</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
@@ -1208,7 +1208,7 @@
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V12" t="inlineStr"/>
@@ -1217,16 +1217,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>67533</v>
+        <v>67569</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>菊莊詩集</t>
+          <t>黃睡漫志</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ju zhuang shi ji</t>
+          <t>huang shui man zhi</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
@@ -1241,7 +1241,7 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K13" t="inlineStr"/>
@@ -1268,7 +1268,7 @@
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V13" t="inlineStr"/>
@@ -1277,16 +1277,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>67534</v>
+        <v>67570</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>琢春詞: 二卷</t>
+          <t>悔人草</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>zuo chun ci</t>
+          <t>hui ren cao</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
@@ -1301,7 +1301,7 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K14" t="inlineStr"/>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V14" t="inlineStr"/>
@@ -1337,16 +1337,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>67535</v>
+        <v>67571</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>蘭雪編年稿</t>
+          <t>舍亭病餘錄</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>lan xue bian nian gao</t>
+          <t>she ting bing yu lu</t>
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
@@ -1361,7 +1361,7 @@
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
@@ -1388,7 +1388,7 @@
       </c>
       <c r="U15" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V15" t="inlineStr"/>
@@ -1397,16 +1397,16 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>67536</v>
+        <v>67572</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>鹿村集</t>
+          <t>汪氏文獻錄</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>lu cun ji</t>
+          <t>wang shi wen xian lu</t>
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
@@ -1421,14 +1421,14 @@
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>15</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -1448,7 +1448,7 @@
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V16" t="inlineStr"/>
@@ -1457,16 +1457,16 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>67537</v>
+        <v>67573</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>隨月樓詩鈔</t>
+          <t>新安紀程</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>sui yue lou shi chao</t>
+          <t>xin an ji cheng</t>
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
@@ -1488,7 +1488,7 @@
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>15</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -1508,7 +1508,7 @@
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V17" t="inlineStr"/>
@@ -1517,16 +1517,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>67538</v>
+        <v>67574</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>晴綺軒詩文集</t>
+          <t>程槐堂詩文集</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>qing qi xuan shi wen ji</t>
+          <t>cheng huai tang shi wen ji</t>
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
@@ -1548,7 +1548,7 @@
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>15</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V18" t="inlineStr"/>
@@ -1577,16 +1577,16 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>67539</v>
+        <v>67575</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>重趼集</t>
+          <t>牀風雨集</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>zhong jian ji</t>
+          <t>chuang feng yu ji</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
@@ -1628,7 +1628,7 @@
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V19" t="inlineStr"/>
@@ -1637,16 +1637,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>67540</v>
+        <v>67576</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>浣雲集</t>
+          <t>粵遊草</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>huan yun ji</t>
+          <t>yue you cao</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V20" t="inlineStr"/>
@@ -1697,16 +1697,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>67541</v>
+        <v>67577</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>楊園遺草: 二卷</t>
+          <t>且隱軒詩集</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>yang yuan yi cao</t>
+          <t>qie yin xuan shi ji</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V21" t="inlineStr"/>
@@ -1757,16 +1757,16 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>67542</v>
+        <v>67578</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>吟息軒詩集</t>
+          <t>懲窒堂集</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>yin xi xuan shi ji</t>
+          <t>cheng zhi tang ji</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
@@ -1808,7 +1808,7 @@
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V22" t="inlineStr"/>
@@ -1817,16 +1817,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>67543</v>
+        <v>67579</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>漁村賸稿</t>
+          <t>拙巢詩集</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>yu cun sheng gao</t>
+          <t>zhuo chao shi ji</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
@@ -1868,7 +1868,7 @@
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V23" t="inlineStr"/>
@@ -1877,16 +1877,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>67544</v>
+        <v>67580</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>梅臯詩草</t>
+          <t>藥蒻園稾</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>mei gao shi cao</t>
+          <t>yao ruo yuan gao</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
@@ -1901,7 +1901,7 @@
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K24" t="inlineStr"/>
@@ -1928,7 +1928,7 @@
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V24" t="inlineStr"/>
@@ -1937,16 +1937,16 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>67545</v>
+        <v>67581</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>杜詩心解</t>
+          <t>沐青樓集</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>du shi xin jie</t>
+          <t>mu qing lou ji</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
@@ -1961,7 +1961,7 @@
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K25" t="inlineStr"/>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V25" t="inlineStr"/>
@@ -1997,16 +1997,16 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>67546</v>
+        <v>67582</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>噓雲稿</t>
+          <t>箕薹詩鈔</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>xu yun gao</t>
+          <t>ji tai shi chao</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
@@ -2021,7 +2021,7 @@
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K26" t="inlineStr"/>
@@ -2048,7 +2048,7 @@
       </c>
       <c r="U26" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V26" t="inlineStr"/>
@@ -2057,16 +2057,16 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>67547</v>
+        <v>67583</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>蝸角攄懷稿</t>
+          <t>蜀游草</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>wo jiao shu huai gao</t>
+          <t>shu you cao</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
@@ -2108,7 +2108,7 @@
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V27" t="inlineStr"/>
@@ -2117,16 +2117,16 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>67548</v>
+        <v>67584</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>安吉堂小草</t>
+          <t>露隱山房詩集</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>an ji tang xiao cao</t>
+          <t>lu yin shan fang shi ji</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V28" t="inlineStr"/>
@@ -2177,16 +2177,16 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>67549</v>
+        <v>67585</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>安定吟草</t>
+          <t>酣隱詩</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>an ding yin cao</t>
+          <t>han yin shi</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
@@ -2201,7 +2201,7 @@
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K29" t="inlineStr"/>
@@ -2228,7 +2228,7 @@
       </c>
       <c r="U29" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V29" t="inlineStr"/>
@@ -2237,16 +2237,16 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>67550</v>
+        <v>67586</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>石門確史</t>
+          <t>宛鳩居詩</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>shi men que shi</t>
+          <t>wan jiu ju shi</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
@@ -2288,7 +2288,7 @@
       </c>
       <c r="U30" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V30" t="inlineStr"/>
@@ -2297,16 +2297,16 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>67551</v>
+        <v>67587</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>滄螺集</t>
+          <t>清輝館集</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>cang luo ji</t>
+          <t>qing hui guan ji</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
@@ -2348,7 +2348,7 @@
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V31" t="inlineStr"/>
@@ -2357,16 +2357,16 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>67552</v>
+        <v>67588</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>笙山草堂詩集</t>
+          <t>梅谷詩鈔</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>sheng shan cao tang shi ji</t>
+          <t>mei gu shi chao</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
@@ -2381,7 +2381,7 @@
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="U32" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V32" t="inlineStr"/>
@@ -2417,16 +2417,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>67553</v>
+        <v>67589</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>一石山房稾</t>
+          <t>夕秀齋詩鈔</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>yi shi shan fang gao</t>
+          <t>xi xiu zhai shi chao</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
@@ -2468,7 +2468,7 @@
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V33" t="inlineStr"/>
@@ -2477,16 +2477,16 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>67554</v>
+        <v>67590</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>春帆集</t>
+          <t>重閬齋詩集</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>chun fan ji</t>
+          <t>zhong lang zhai shi ji</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
@@ -2528,7 +2528,7 @@
       </c>
       <c r="U34" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V34" t="inlineStr"/>
@@ -2537,16 +2537,16 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>67555</v>
+        <v>67591</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>拳石齋詩集</t>
+          <t>北溪草堂吟稾</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>quan shi zhai shi ji</t>
+          <t>bei xi cao tang yin gao</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
@@ -2561,7 +2561,7 @@
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V35" t="inlineStr"/>
@@ -2597,16 +2597,16 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>67556</v>
+        <v>67592</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>學田集</t>
+          <t>寒綠齋詩集</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>xue tian ji</t>
+          <t>han lv zhai shi ji</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
@@ -2648,12 +2648,1752 @@
       </c>
       <c r="U36" t="inlineStr">
         <is>
-          <t>20241213</t>
+          <t>20241220</t>
         </is>
       </c>
       <c r="V36" t="inlineStr"/>
       <c r="W36" t="inlineStr"/>
       <c r="X36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>67593</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>京口遺音集</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>jing kou yi yin ji</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr"/>
+      <c r="R37" t="inlineStr"/>
+      <c r="S37" t="inlineStr"/>
+      <c r="T37" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V37" t="inlineStr"/>
+      <c r="W37" t="inlineStr"/>
+      <c r="X37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>67594</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>澡雪吟稾</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>zao xue yin gao</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
+      <c r="Q38" t="inlineStr"/>
+      <c r="R38" t="inlineStr"/>
+      <c r="S38" t="inlineStr"/>
+      <c r="T38" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V38" t="inlineStr"/>
+      <c r="W38" t="inlineStr"/>
+      <c r="X38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>67595</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>澄秋閣詩集: 十二卷</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>cheng qiu ge shi ji</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
+      <c r="Q39" t="inlineStr"/>
+      <c r="R39" t="inlineStr"/>
+      <c r="S39" t="inlineStr"/>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V39" t="inlineStr"/>
+      <c r="W39" t="inlineStr"/>
+      <c r="X39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>67596</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>論山詩文集</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>lun shan shi wen ji</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
+      <c r="Q40" t="inlineStr"/>
+      <c r="R40" t="inlineStr"/>
+      <c r="S40" t="inlineStr"/>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V40" t="inlineStr"/>
+      <c r="W40" t="inlineStr"/>
+      <c r="X40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>67597</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>小齊雲山館詩鈔</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>xiao qi yun shan guan shi chao</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="inlineStr"/>
+      <c r="S41" t="inlineStr"/>
+      <c r="T41" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
+      <c r="X41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>67598</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>花韻山房集</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>hua yun shan fang ji</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr"/>
+      <c r="R42" t="inlineStr"/>
+      <c r="S42" t="inlineStr"/>
+      <c r="T42" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V42" t="inlineStr"/>
+      <c r="W42" t="inlineStr"/>
+      <c r="X42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>67599</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>白首江上集</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>bai shou jiang shang ji</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
+      <c r="R43" t="inlineStr"/>
+      <c r="S43" t="inlineStr"/>
+      <c r="T43" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
+      <c r="X43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>67600</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>晨村集</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>chen cun ji</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
+      <c r="R44" t="inlineStr"/>
+      <c r="S44" t="inlineStr"/>
+      <c r="T44" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V44" t="inlineStr"/>
+      <c r="W44" t="inlineStr"/>
+      <c r="X44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>67601</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>櫧山艸堂詩稾</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>zhu shan cao tang shi gao</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr"/>
+      <c r="R45" t="inlineStr"/>
+      <c r="S45" t="inlineStr"/>
+      <c r="T45" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V45" t="inlineStr"/>
+      <c r="W45" t="inlineStr"/>
+      <c r="X45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>67602</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>寄漚閒舫詩鈔</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>ji ou xian fang shi chao</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
+      <c r="Q46" t="inlineStr"/>
+      <c r="R46" t="inlineStr"/>
+      <c r="S46" t="inlineStr"/>
+      <c r="T46" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V46" t="inlineStr"/>
+      <c r="W46" t="inlineStr"/>
+      <c r="X46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>67603</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>宜秋閣詩鈔</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>yi qiu ge shi chao</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr"/>
+      <c r="R47" t="inlineStr"/>
+      <c r="S47" t="inlineStr"/>
+      <c r="T47" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V47" t="inlineStr"/>
+      <c r="W47" t="inlineStr"/>
+      <c r="X47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>67604</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>雙梧集</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>shuang wu ji</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>2067</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
+      <c r="Q48" t="inlineStr"/>
+      <c r="R48" t="inlineStr"/>
+      <c r="S48" t="inlineStr"/>
+      <c r="T48" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V48" t="inlineStr"/>
+      <c r="W48" t="inlineStr"/>
+      <c r="X48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>67605</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>恬齋遺詩</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>tian zhai yi shi</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
+      <c r="Q49" t="inlineStr"/>
+      <c r="R49" t="inlineStr"/>
+      <c r="S49" t="inlineStr"/>
+      <c r="T49" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V49" t="inlineStr"/>
+      <c r="W49" t="inlineStr"/>
+      <c r="X49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>67606</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>青棠館詩集</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>qing tang guan shi ji</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
+      <c r="Q50" t="inlineStr"/>
+      <c r="R50" t="inlineStr"/>
+      <c r="S50" t="inlineStr"/>
+      <c r="T50" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V50" t="inlineStr"/>
+      <c r="W50" t="inlineStr"/>
+      <c r="X50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>67607</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>秋浦詩鈔</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>qiu pu shi chao</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
+      <c r="Q51" t="inlineStr"/>
+      <c r="R51" t="inlineStr"/>
+      <c r="S51" t="inlineStr"/>
+      <c r="T51" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V51" t="inlineStr"/>
+      <c r="W51" t="inlineStr"/>
+      <c r="X51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>67608</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>澹芷詩鈔</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>dan zhi shi chao</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
+      <c r="Q52" t="inlineStr"/>
+      <c r="R52" t="inlineStr"/>
+      <c r="S52" t="inlineStr"/>
+      <c r="T52" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V52" t="inlineStr"/>
+      <c r="W52" t="inlineStr"/>
+      <c r="X52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>67609</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>六觀齋詩集</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>liu guan zhai shi ji</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
+      <c r="Q53" t="inlineStr"/>
+      <c r="R53" t="inlineStr"/>
+      <c r="S53" t="inlineStr"/>
+      <c r="T53" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V53" t="inlineStr"/>
+      <c r="W53" t="inlineStr"/>
+      <c r="X53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>67610</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>扶雲館詩</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>fu yun guan shi</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
+      <c r="Q54" t="inlineStr"/>
+      <c r="R54" t="inlineStr"/>
+      <c r="S54" t="inlineStr"/>
+      <c r="T54" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U54" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V54" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>67611</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>玉句草堂詩集</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>yu ju cao tang shi ji</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
+      <c r="Q55" t="inlineStr"/>
+      <c r="R55" t="inlineStr"/>
+      <c r="S55" t="inlineStr"/>
+      <c r="T55" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V55" t="inlineStr"/>
+      <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>67612</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>抱山堂詩選</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>bao shan tang shi xuan</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
+      <c r="R56" t="inlineStr"/>
+      <c r="S56" t="inlineStr"/>
+      <c r="T56" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V56" t="inlineStr"/>
+      <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>67613</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>持雅堂集</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>chi ya tang ji</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
+      <c r="Q57" t="inlineStr"/>
+      <c r="R57" t="inlineStr"/>
+      <c r="S57" t="inlineStr"/>
+      <c r="T57" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>67614</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>味餘樓集</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>wei yu lou ji</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
+      <c r="R58" t="inlineStr"/>
+      <c r="S58" t="inlineStr"/>
+      <c r="T58" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V58" t="inlineStr"/>
+      <c r="W58" t="inlineStr"/>
+      <c r="X58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>67615</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>湘雪軒詩</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>xiang xue xuan shi</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr"/>
+      <c r="R59" t="inlineStr"/>
+      <c r="S59" t="inlineStr"/>
+      <c r="T59" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V59" t="inlineStr"/>
+      <c r="W59" t="inlineStr"/>
+      <c r="X59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>67616</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>富溪眺詠集</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>fu xi tiao yong ji</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr"/>
+      <c r="R60" t="inlineStr"/>
+      <c r="S60" t="inlineStr"/>
+      <c r="T60" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V60" t="inlineStr"/>
+      <c r="W60" t="inlineStr"/>
+      <c r="X60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>67617</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>聽松樓詩</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>ting song lou shi</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr"/>
+      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
+      <c r="Q61" t="inlineStr"/>
+      <c r="R61" t="inlineStr"/>
+      <c r="S61" t="inlineStr"/>
+      <c r="T61" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V61" t="inlineStr"/>
+      <c r="W61" t="inlineStr"/>
+      <c r="X61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>67618</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>雙蟾閣詩</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>shuang chan ge shi</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr"/>
+      <c r="R62" t="inlineStr"/>
+      <c r="S62" t="inlineStr"/>
+      <c r="T62" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V62" t="inlineStr"/>
+      <c r="W62" t="inlineStr"/>
+      <c r="X62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>67619</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>詅癡集</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>ling chi ji</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
+      <c r="Q63" t="inlineStr"/>
+      <c r="R63" t="inlineStr"/>
+      <c r="S63" t="inlineStr"/>
+      <c r="T63" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V63" t="inlineStr"/>
+      <c r="W63" t="inlineStr"/>
+      <c r="X63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>67620</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>江湖載酒吟</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>jiang hu zai jiu yin</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr"/>
+      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
+      <c r="Q64" t="inlineStr"/>
+      <c r="R64" t="inlineStr"/>
+      <c r="S64" t="inlineStr"/>
+      <c r="T64" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V64" t="inlineStr"/>
+      <c r="W64" t="inlineStr"/>
+      <c r="X64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>67621</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>憑山草堂集</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>ping shan cao tang ji</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr"/>
+      <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>65192</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr"/>
+      <c r="P65" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
+      <c r="R65" t="inlineStr"/>
+      <c r="S65" t="inlineStr"/>
+      <c r="T65" t="inlineStr">
+        <is>
+          <t>load</t>
+        </is>
+      </c>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>20241220</t>
+        </is>
+      </c>
+      <c r="V65" t="inlineStr"/>
+      <c r="W65" t="inlineStr"/>
+      <c r="X65" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>